<commit_message>
all under 10 table
</commit_message>
<xml_diff>
--- a/results/comparison_table/Fishers_comparison.xlsx
+++ b/results/comparison_table/Fishers_comparison.xlsx
@@ -659,7 +659,7 @@
         <v>0.3773962335319018</v>
       </c>
       <c r="D4" s="14" t="n">
-        <v>9.919356917703732</v>
+        <v>7.44685327999801</v>
       </c>
       <c r="E4" s="14" t="n">
         <v>4.689288745604718</v>
@@ -678,7 +678,7 @@
         <v>0.35284833961881</v>
       </c>
       <c r="K4" s="14" t="n">
-        <v>4.304025912258477</v>
+        <v>1.638660234711782</v>
       </c>
       <c r="L4" s="14" t="n">
         <v>4.689288745605105</v>
@@ -709,7 +709,7 @@
       </c>
       <c r="C5" s="14" t="n"/>
       <c r="D5" s="14" t="n">
-        <v>9.886936539789014</v>
+        <v>7.402409024285747</v>
       </c>
       <c r="E5" s="14" t="n">
         <v>4.719477185936323</v>
@@ -728,7 +728,7 @@
       </c>
       <c r="J5" s="14" t="n"/>
       <c r="K5" s="14" t="n">
-        <v>3.981254205101203</v>
+        <v>1.630821204415821</v>
       </c>
       <c r="L5" s="14" t="n">
         <v>4.719477185933972</v>
@@ -755,17 +755,17 @@
         </is>
       </c>
       <c r="B6" s="14" t="n">
-        <v>9.919356917703732</v>
+        <v>7.44685327999801</v>
       </c>
       <c r="C6" s="14" t="n">
-        <v>9.886936539789014</v>
+        <v>7.402409024285747</v>
       </c>
       <c r="D6" s="14" t="n"/>
       <c r="E6" s="14" t="n">
-        <v>7.117976427563766</v>
+        <v>7.508599766439922</v>
       </c>
       <c r="F6" s="14" t="n">
-        <v>9.99217094197501</v>
+        <v>7.43725906158682</v>
       </c>
       <c r="G6" s="13" t="n"/>
       <c r="H6" s="12" t="inlineStr">
@@ -774,17 +774,17 @@
         </is>
       </c>
       <c r="I6" s="14" t="n">
-        <v>4.304025912258477</v>
+        <v>1.638660234711782</v>
       </c>
       <c r="J6" s="14" t="n">
-        <v>3.981254205101203</v>
+        <v>1.630821204415821</v>
       </c>
       <c r="K6" s="14" t="n"/>
       <c r="L6" s="14" t="n">
-        <v>5.106398705457906</v>
+        <v>5.150636344937815</v>
       </c>
       <c r="M6" s="14" t="n">
-        <v>3.930611463694983</v>
+        <v>1.657017485361074</v>
       </c>
       <c r="N6" s="13" t="n"/>
       <c r="O6" s="13" t="n"/>
@@ -811,7 +811,7 @@
         <v>4.719477185936323</v>
       </c>
       <c r="D7" s="14" t="n">
-        <v>7.117976427563766</v>
+        <v>7.508599766439922</v>
       </c>
       <c r="E7" s="14" t="n"/>
       <c r="F7" s="14" t="n">
@@ -830,7 +830,7 @@
         <v>4.719477185933972</v>
       </c>
       <c r="K7" s="14" t="n">
-        <v>5.106398705457906</v>
+        <v>5.150636344937815</v>
       </c>
       <c r="L7" s="14" t="n"/>
       <c r="M7" s="14" t="n">
@@ -861,7 +861,7 @@
         <v>0.1761392290294239</v>
       </c>
       <c r="D8" s="14" t="n">
-        <v>9.99217094197501</v>
+        <v>7.43725906158682</v>
       </c>
       <c r="E8" s="14" t="n">
         <v>4.708879397782754</v>
@@ -879,7 +879,7 @@
         <v>0.2314736072303805</v>
       </c>
       <c r="K8" s="14" t="n">
-        <v>3.930611463694983</v>
+        <v>1.657017485361074</v>
       </c>
       <c r="L8" s="14" t="n">
         <v>4.7088793977721</v>
@@ -995,7 +995,7 @@
         <v>0.377396233533012</v>
       </c>
       <c r="D14" s="14" t="n">
-        <v>9.919356917702338</v>
+        <v>7.446853279991807</v>
       </c>
       <c r="E14" s="14" t="n">
         <v>3.186027703199337</v>
@@ -1013,7 +1013,7 @@
         <v>0.002445764974182504</v>
       </c>
       <c r="K14" s="14" t="n">
-        <v>4.264097540967208</v>
+        <v>1.251583407461542</v>
       </c>
       <c r="L14" s="14" t="n">
         <v>0.005067295447965768</v>
@@ -1033,7 +1033,7 @@
       </c>
       <c r="C15" s="14" t="n"/>
       <c r="D15" s="14" t="n">
-        <v>9.886936539793002</v>
+        <v>7.402409024286854</v>
       </c>
       <c r="E15" s="14" t="n">
         <v>3.15331911680175</v>
@@ -1051,7 +1051,7 @@
       </c>
       <c r="J15" s="14" t="n"/>
       <c r="K15" s="14" t="n">
-        <v>4.265870609220072</v>
+        <v>1.251648196523142</v>
       </c>
       <c r="L15" s="14" t="n">
         <v>0.003617750813900871</v>
@@ -1067,17 +1067,17 @@
         </is>
       </c>
       <c r="B16" s="14" t="n">
-        <v>9.919356917702338</v>
+        <v>7.446853279991807</v>
       </c>
       <c r="C16" s="14" t="n">
-        <v>9.886936539793002</v>
+        <v>7.402409024286854</v>
       </c>
       <c r="D16" s="14" t="n"/>
       <c r="E16" s="14" t="n">
-        <v>7.117976427563251</v>
+        <v>7.508599766440905</v>
       </c>
       <c r="F16" s="14" t="n">
-        <v>9.992170941966545</v>
+        <v>7.43725906158266</v>
       </c>
       <c r="H16" s="12" t="inlineStr">
         <is>
@@ -1085,17 +1085,17 @@
         </is>
       </c>
       <c r="I16" s="14" t="n">
-        <v>4.264097540967208</v>
+        <v>1.251583407461542</v>
       </c>
       <c r="J16" s="14" t="n">
-        <v>4.265870609220072</v>
+        <v>1.251648196523142</v>
       </c>
       <c r="K16" s="14" t="n"/>
       <c r="L16" s="14" t="n">
-        <v>4.269155611861901</v>
+        <v>1.249225073247281</v>
       </c>
       <c r="M16" s="14" t="n">
-        <v>4.26838847448473</v>
+        <v>1.250475563523044</v>
       </c>
     </row>
     <row r="17" ht="15.85" customHeight="1" s="10">
@@ -1111,7 +1111,7 @@
         <v>3.15331911680175</v>
       </c>
       <c r="D17" s="14" t="n">
-        <v>7.117976427563251</v>
+        <v>7.508599766440905</v>
       </c>
       <c r="E17" s="14" t="n"/>
       <c r="F17" s="14" t="n">
@@ -1129,7 +1129,7 @@
         <v>0.003617750813900871</v>
       </c>
       <c r="K17" s="14" t="n">
-        <v>4.269155611861901</v>
+        <v>1.249225073247281</v>
       </c>
       <c r="L17" s="14" t="n"/>
       <c r="M17" s="14" t="n">
@@ -1149,7 +1149,7 @@
         <v>0.1761392290301824</v>
       </c>
       <c r="D18" s="14" t="n">
-        <v>9.992170941966545</v>
+        <v>7.43725906158266</v>
       </c>
       <c r="E18" s="14" t="n">
         <v>3.259494281966406</v>
@@ -1167,7 +1167,7 @@
         <v>0.002821980829311123</v>
       </c>
       <c r="K18" s="14" t="n">
-        <v>4.26838847448473</v>
+        <v>1.250475563523044</v>
       </c>
       <c r="L18" s="14" t="n">
         <v>0.001250791272115822</v>
@@ -1367,7 +1367,7 @@
         <v>0.3726463025137923</v>
       </c>
       <c r="D4" s="14" t="n">
-        <v>10.84289138992081</v>
+        <v>3.384266125046481</v>
       </c>
       <c r="E4" s="14" t="n">
         <v>1.173174098906264</v>
@@ -1386,7 +1386,7 @@
         <v>0.4491435128481215</v>
       </c>
       <c r="K4" s="14" t="n">
-        <v>2.614010165875955</v>
+        <v>1.189449767637524</v>
       </c>
       <c r="L4" s="14" t="n">
         <v>2.865230972178754</v>
@@ -1417,7 +1417,7 @@
       </c>
       <c r="C5" s="14" t="n"/>
       <c r="D5" s="14" t="n">
-        <v>10.8728026011959</v>
+        <v>3.918593313466014</v>
       </c>
       <c r="E5" s="14" t="n">
         <v>1.314870456468473</v>
@@ -1436,7 +1436,7 @@
       </c>
       <c r="J5" s="14" t="n"/>
       <c r="K5" s="14" t="n">
-        <v>2.625541679111308</v>
+        <v>1.202402704743217</v>
       </c>
       <c r="L5" s="14" t="n">
         <v>2.88437463456303</v>
@@ -1463,17 +1463,17 @@
         </is>
       </c>
       <c r="B6" s="14" t="n">
-        <v>10.84289138992081</v>
+        <v>3.384266125046481</v>
       </c>
       <c r="C6" s="14" t="n">
-        <v>10.8728026011959</v>
+        <v>3.918593313466014</v>
       </c>
       <c r="D6" s="14" t="n"/>
       <c r="E6" s="14" t="n">
-        <v>10.30055688556166</v>
+        <v>4.242445508897008</v>
       </c>
       <c r="F6" s="14" t="n">
-        <v>10.84918233753177</v>
+        <v>3.402226655773111</v>
       </c>
       <c r="G6" s="13" t="n"/>
       <c r="H6" s="12" t="inlineStr">
@@ -1482,17 +1482,17 @@
         </is>
       </c>
       <c r="I6" s="14" t="n">
-        <v>2.614010165875955</v>
+        <v>1.189449767637524</v>
       </c>
       <c r="J6" s="14" t="n">
-        <v>2.625541679111308</v>
+        <v>1.202402704743217</v>
       </c>
       <c r="K6" s="14" t="n"/>
       <c r="L6" s="14" t="n">
-        <v>3.210258439842438</v>
+        <v>1.636833993271819</v>
       </c>
       <c r="M6" s="14" t="n">
-        <v>2.617148387586216</v>
+        <v>1.269127300816686</v>
       </c>
       <c r="N6" s="13" t="n"/>
       <c r="O6" s="13" t="n"/>
@@ -1519,7 +1519,7 @@
         <v>1.314870456468473</v>
       </c>
       <c r="D7" s="14" t="n">
-        <v>10.30055688556166</v>
+        <v>4.242445508897008</v>
       </c>
       <c r="E7" s="14" t="n"/>
       <c r="F7" s="14" t="n">
@@ -1538,7 +1538,7 @@
         <v>2.88437463456303</v>
       </c>
       <c r="K7" s="14" t="n">
-        <v>3.210258439842438</v>
+        <v>1.636833993271819</v>
       </c>
       <c r="L7" s="14" t="n"/>
       <c r="M7" s="14" t="n">
@@ -1569,7 +1569,7 @@
         <v>0.1081616267389053</v>
       </c>
       <c r="D8" s="14" t="n">
-        <v>10.84918233753177</v>
+        <v>3.402226655773111</v>
       </c>
       <c r="E8" s="14" t="n">
         <v>1.260488548518442</v>
@@ -1587,7 +1587,7 @@
         <v>0.1392586598233071</v>
       </c>
       <c r="K8" s="14" t="n">
-        <v>2.617148387586216</v>
+        <v>1.269127300816686</v>
       </c>
       <c r="L8" s="14" t="n">
         <v>2.97560847582311</v>
@@ -1703,7 +1703,7 @@
         <v>0.3726463025141316</v>
       </c>
       <c r="D14" s="14" t="n">
-        <v>10.84289138992082</v>
+        <v>3.38426612505494</v>
       </c>
       <c r="E14" s="14" t="n">
         <v>2.081437496736004</v>
@@ -1721,7 +1721,7 @@
         <v>0.004883347111689611</v>
       </c>
       <c r="K14" s="14" t="n">
-        <v>3.453247927247328</v>
+        <v>1.592455224818253</v>
       </c>
       <c r="L14" s="14" t="n">
         <v>0.005149342423874624</v>
@@ -1741,7 +1741,7 @@
       </c>
       <c r="C15" s="14" t="n"/>
       <c r="D15" s="14" t="n">
-        <v>10.87280260119602</v>
+        <v>3.62054734826109</v>
       </c>
       <c r="E15" s="14" t="n">
         <v>2.106366134259678</v>
@@ -1759,7 +1759,7 @@
       </c>
       <c r="J15" s="14" t="n"/>
       <c r="K15" s="14" t="n">
-        <v>3.453996048594282</v>
+        <v>4.097090025903984</v>
       </c>
       <c r="L15" s="14" t="n">
         <v>0.001263305374658307</v>
@@ -1775,17 +1775,17 @@
         </is>
       </c>
       <c r="B16" s="14" t="n">
-        <v>10.84289138992082</v>
+        <v>3.38426612505494</v>
       </c>
       <c r="C16" s="14" t="n">
-        <v>10.87280260119602</v>
+        <v>3.62054734826109</v>
       </c>
       <c r="D16" s="14" t="n"/>
       <c r="E16" s="14" t="n">
-        <v>10.30055688556187</v>
+        <v>4.242445508900473</v>
       </c>
       <c r="F16" s="14" t="n">
-        <v>10.84918233753237</v>
+        <v>3.402226655778946</v>
       </c>
       <c r="H16" s="12" t="inlineStr">
         <is>
@@ -1793,17 +1793,17 @@
         </is>
       </c>
       <c r="I16" s="14" t="n">
-        <v>3.453247927247328</v>
+        <v>1.592455224818253</v>
       </c>
       <c r="J16" s="14" t="n">
-        <v>3.453996048594282</v>
+        <v>4.097090025903984</v>
       </c>
       <c r="K16" s="14" t="n"/>
       <c r="L16" s="14" t="n">
-        <v>3.437629267924787</v>
+        <v>4.09713449033247</v>
       </c>
       <c r="M16" s="14" t="n">
-        <v>3.454313084573598</v>
+        <v>1.597460369086457</v>
       </c>
     </row>
     <row r="17" ht="15.85" customHeight="1" s="10">
@@ -1819,7 +1819,7 @@
         <v>2.106366134259678</v>
       </c>
       <c r="D17" s="14" t="n">
-        <v>10.30055688556187</v>
+        <v>4.242445508900473</v>
       </c>
       <c r="E17" s="14" t="n"/>
       <c r="F17" s="14" t="n">
@@ -1837,7 +1837,7 @@
         <v>0.001263305374658307</v>
       </c>
       <c r="K17" s="14" t="n">
-        <v>3.437629267924787</v>
+        <v>4.09713449033247</v>
       </c>
       <c r="L17" s="14" t="n"/>
       <c r="M17" s="14" t="n">
@@ -1857,7 +1857,7 @@
         <v>0.1081616267395801</v>
       </c>
       <c r="D18" s="14" t="n">
-        <v>10.84918233753237</v>
+        <v>3.402226655778946</v>
       </c>
       <c r="E18" s="14" t="n">
         <v>2.104415939014535</v>
@@ -1875,7 +1875,7 @@
         <v>0.001359305145372738</v>
       </c>
       <c r="K18" s="14" t="n">
-        <v>3.454313084573598</v>
+        <v>1.597460369086457</v>
       </c>
       <c r="L18" s="14" t="n">
         <v>0.001075452800861554</v>

</xml_diff>

<commit_message>
updated table with updated output of spec-opt
</commit_message>
<xml_diff>
--- a/results/comparison_table/Fishers_comparison.xlsx
+++ b/results/comparison_table/Fishers_comparison.xlsx
@@ -659,7 +659,7 @@
         <v>0.3773962335319018</v>
       </c>
       <c r="D4" s="14" t="n">
-        <v>7.44685327999801</v>
+        <v>9.919356917703732</v>
       </c>
       <c r="E4" s="14" t="n">
         <v>4.689288745604718</v>
@@ -678,7 +678,7 @@
         <v>0.35284833961881</v>
       </c>
       <c r="K4" s="14" t="n">
-        <v>1.638660234711782</v>
+        <v>4.304025912258477</v>
       </c>
       <c r="L4" s="14" t="n">
         <v>4.689288745605105</v>
@@ -709,7 +709,7 @@
       </c>
       <c r="C5" s="14" t="n"/>
       <c r="D5" s="14" t="n">
-        <v>7.402409024285747</v>
+        <v>9.886936539789014</v>
       </c>
       <c r="E5" s="14" t="n">
         <v>4.719477185936323</v>
@@ -728,7 +728,7 @@
       </c>
       <c r="J5" s="14" t="n"/>
       <c r="K5" s="14" t="n">
-        <v>1.630821204415821</v>
+        <v>3.981254205101203</v>
       </c>
       <c r="L5" s="14" t="n">
         <v>4.719477185933972</v>
@@ -755,17 +755,17 @@
         </is>
       </c>
       <c r="B6" s="14" t="n">
-        <v>7.44685327999801</v>
+        <v>9.919356917703732</v>
       </c>
       <c r="C6" s="14" t="n">
-        <v>7.402409024285747</v>
+        <v>9.886936539789014</v>
       </c>
       <c r="D6" s="14" t="n"/>
       <c r="E6" s="14" t="n">
-        <v>7.508599766439922</v>
+        <v>7.117976427563766</v>
       </c>
       <c r="F6" s="14" t="n">
-        <v>7.43725906158682</v>
+        <v>9.99217094197501</v>
       </c>
       <c r="G6" s="13" t="n"/>
       <c r="H6" s="12" t="inlineStr">
@@ -774,17 +774,17 @@
         </is>
       </c>
       <c r="I6" s="14" t="n">
-        <v>1.638660234711782</v>
+        <v>4.304025912258477</v>
       </c>
       <c r="J6" s="14" t="n">
-        <v>1.630821204415821</v>
+        <v>3.981254205101203</v>
       </c>
       <c r="K6" s="14" t="n"/>
       <c r="L6" s="14" t="n">
-        <v>5.150636344937815</v>
+        <v>5.106398705457906</v>
       </c>
       <c r="M6" s="14" t="n">
-        <v>1.657017485361074</v>
+        <v>3.930611463694983</v>
       </c>
       <c r="N6" s="13" t="n"/>
       <c r="O6" s="13" t="n"/>
@@ -811,7 +811,7 @@
         <v>4.719477185936323</v>
       </c>
       <c r="D7" s="14" t="n">
-        <v>7.508599766439922</v>
+        <v>7.117976427563766</v>
       </c>
       <c r="E7" s="14" t="n"/>
       <c r="F7" s="14" t="n">
@@ -830,7 +830,7 @@
         <v>4.719477185933972</v>
       </c>
       <c r="K7" s="14" t="n">
-        <v>5.150636344937815</v>
+        <v>5.106398705457906</v>
       </c>
       <c r="L7" s="14" t="n"/>
       <c r="M7" s="14" t="n">
@@ -861,7 +861,7 @@
         <v>0.1761392290294239</v>
       </c>
       <c r="D8" s="14" t="n">
-        <v>7.43725906158682</v>
+        <v>9.99217094197501</v>
       </c>
       <c r="E8" s="14" t="n">
         <v>4.708879397782754</v>
@@ -879,7 +879,7 @@
         <v>0.2314736072303805</v>
       </c>
       <c r="K8" s="14" t="n">
-        <v>1.657017485361074</v>
+        <v>3.930611463694983</v>
       </c>
       <c r="L8" s="14" t="n">
         <v>4.7088793977721</v>
@@ -995,7 +995,7 @@
         <v>0.377396233533012</v>
       </c>
       <c r="D14" s="14" t="n">
-        <v>7.446853279991807</v>
+        <v>9.919356917702338</v>
       </c>
       <c r="E14" s="14" t="n">
         <v>3.186027703199337</v>
@@ -1013,7 +1013,7 @@
         <v>0.002445764974182504</v>
       </c>
       <c r="K14" s="14" t="n">
-        <v>1.251583407461542</v>
+        <v>4.264097540967208</v>
       </c>
       <c r="L14" s="14" t="n">
         <v>0.005067295447965768</v>
@@ -1033,7 +1033,7 @@
       </c>
       <c r="C15" s="14" t="n"/>
       <c r="D15" s="14" t="n">
-        <v>7.402409024286854</v>
+        <v>9.886936539793002</v>
       </c>
       <c r="E15" s="14" t="n">
         <v>3.15331911680175</v>
@@ -1051,7 +1051,7 @@
       </c>
       <c r="J15" s="14" t="n"/>
       <c r="K15" s="14" t="n">
-        <v>1.251648196523142</v>
+        <v>4.265870609220072</v>
       </c>
       <c r="L15" s="14" t="n">
         <v>0.003617750813900871</v>
@@ -1067,17 +1067,17 @@
         </is>
       </c>
       <c r="B16" s="14" t="n">
-        <v>7.446853279991807</v>
+        <v>9.919356917702338</v>
       </c>
       <c r="C16" s="14" t="n">
-        <v>7.402409024286854</v>
+        <v>9.886936539793002</v>
       </c>
       <c r="D16" s="14" t="n"/>
       <c r="E16" s="14" t="n">
-        <v>7.508599766440905</v>
+        <v>7.117976427563251</v>
       </c>
       <c r="F16" s="14" t="n">
-        <v>7.43725906158266</v>
+        <v>9.992170941966545</v>
       </c>
       <c r="H16" s="12" t="inlineStr">
         <is>
@@ -1085,17 +1085,17 @@
         </is>
       </c>
       <c r="I16" s="14" t="n">
-        <v>1.251583407461542</v>
+        <v>4.264097540967208</v>
       </c>
       <c r="J16" s="14" t="n">
-        <v>1.251648196523142</v>
+        <v>4.265870609220072</v>
       </c>
       <c r="K16" s="14" t="n"/>
       <c r="L16" s="14" t="n">
-        <v>1.249225073247281</v>
+        <v>4.269155611861901</v>
       </c>
       <c r="M16" s="14" t="n">
-        <v>1.250475563523044</v>
+        <v>4.26838847448473</v>
       </c>
     </row>
     <row r="17" ht="15.85" customHeight="1" s="10">
@@ -1111,7 +1111,7 @@
         <v>3.15331911680175</v>
       </c>
       <c r="D17" s="14" t="n">
-        <v>7.508599766440905</v>
+        <v>7.117976427563251</v>
       </c>
       <c r="E17" s="14" t="n"/>
       <c r="F17" s="14" t="n">
@@ -1129,7 +1129,7 @@
         <v>0.003617750813900871</v>
       </c>
       <c r="K17" s="14" t="n">
-        <v>1.249225073247281</v>
+        <v>4.269155611861901</v>
       </c>
       <c r="L17" s="14" t="n"/>
       <c r="M17" s="14" t="n">
@@ -1149,7 +1149,7 @@
         <v>0.1761392290301824</v>
       </c>
       <c r="D18" s="14" t="n">
-        <v>7.43725906158266</v>
+        <v>9.992170941966545</v>
       </c>
       <c r="E18" s="14" t="n">
         <v>3.259494281966406</v>
@@ -1167,7 +1167,7 @@
         <v>0.002821980829311123</v>
       </c>
       <c r="K18" s="14" t="n">
-        <v>1.250475563523044</v>
+        <v>4.26838847448473</v>
       </c>
       <c r="L18" s="14" t="n">
         <v>0.001250791272115822</v>
@@ -1473,7 +1473,7 @@
         <v>4.242445508897008</v>
       </c>
       <c r="F6" s="14" t="n">
-        <v>3.402226655773111</v>
+        <v>10.84918233753177</v>
       </c>
       <c r="G6" s="13" t="n"/>
       <c r="H6" s="12" t="inlineStr">
@@ -1492,7 +1492,7 @@
         <v>1.636833993271819</v>
       </c>
       <c r="M6" s="14" t="n">
-        <v>1.269127300816686</v>
+        <v>2.617148387586216</v>
       </c>
       <c r="N6" s="13" t="n"/>
       <c r="O6" s="13" t="n"/>
@@ -1569,7 +1569,7 @@
         <v>0.1081616267389053</v>
       </c>
       <c r="D8" s="14" t="n">
-        <v>3.402226655773111</v>
+        <v>10.84918233753177</v>
       </c>
       <c r="E8" s="14" t="n">
         <v>1.260488548518442</v>
@@ -1587,7 +1587,7 @@
         <v>0.1392586598233071</v>
       </c>
       <c r="K8" s="14" t="n">
-        <v>1.269127300816686</v>
+        <v>2.617148387586216</v>
       </c>
       <c r="L8" s="14" t="n">
         <v>2.97560847582311</v>
@@ -1785,7 +1785,7 @@
         <v>4.242445508900473</v>
       </c>
       <c r="F16" s="14" t="n">
-        <v>3.402226655778946</v>
+        <v>10.84918233753237</v>
       </c>
       <c r="H16" s="12" t="inlineStr">
         <is>
@@ -1803,7 +1803,7 @@
         <v>4.09713449033247</v>
       </c>
       <c r="M16" s="14" t="n">
-        <v>1.597460369086457</v>
+        <v>3.454313084573598</v>
       </c>
     </row>
     <row r="17" ht="15.85" customHeight="1" s="10">
@@ -1857,7 +1857,7 @@
         <v>0.1081616267395801</v>
       </c>
       <c r="D18" s="14" t="n">
-        <v>3.402226655778946</v>
+        <v>10.84918233753237</v>
       </c>
       <c r="E18" s="14" t="n">
         <v>2.104415939014535</v>
@@ -1875,7 +1875,7 @@
         <v>0.001359305145372738</v>
       </c>
       <c r="K18" s="14" t="n">
-        <v>1.597460369086457</v>
+        <v>3.454313084573598</v>
       </c>
       <c r="L18" s="14" t="n">
         <v>0.001075452800861554</v>
@@ -2075,7 +2075,7 @@
         <v>0.2262904584537549</v>
       </c>
       <c r="D4" s="14" t="n">
-        <v>9.041864007425653</v>
+        <v>5.469262880664999</v>
       </c>
       <c r="E4" s="14" t="n">
         <v>2.701114701640339</v>
@@ -2094,7 +2094,7 @@
         <v>0.09070967271611728</v>
       </c>
       <c r="K4" s="14" t="n">
-        <v>12.42479335229207</v>
+        <v>4.519503360644053</v>
       </c>
       <c r="L4" s="14" t="n">
         <v>2.274282554125683</v>
@@ -2125,7 +2125,7 @@
       </c>
       <c r="C5" s="14" t="n"/>
       <c r="D5" s="14" t="n">
-        <v>9.073006014803994</v>
+        <v>5.497487840891996</v>
       </c>
       <c r="E5" s="14" t="n">
         <v>2.844001213689403</v>
@@ -2144,7 +2144,7 @@
       </c>
       <c r="J5" s="14" t="n"/>
       <c r="K5" s="14" t="n">
-        <v>12.42567251460646</v>
+        <v>4.524026768922548</v>
       </c>
       <c r="L5" s="14" t="n">
         <v>2.296414533926163</v>
@@ -2171,17 +2171,17 @@
         </is>
       </c>
       <c r="B6" s="14" t="n">
-        <v>9.041864007425653</v>
+        <v>5.469262880664999</v>
       </c>
       <c r="C6" s="14" t="n">
-        <v>9.073006014803994</v>
+        <v>5.497487840891996</v>
       </c>
       <c r="D6" s="14" t="n"/>
       <c r="E6" s="14" t="n">
-        <v>9.703072181449262</v>
+        <v>5.328235491198823</v>
       </c>
       <c r="F6" s="14" t="n">
-        <v>8.960981046584797</v>
+        <v>5.458721538855309</v>
       </c>
       <c r="G6" s="13" t="n"/>
       <c r="H6" s="12" t="inlineStr">
@@ -2190,17 +2190,17 @@
         </is>
       </c>
       <c r="I6" s="14" t="n">
-        <v>12.42479335229207</v>
+        <v>4.519503360644053</v>
       </c>
       <c r="J6" s="14" t="n">
-        <v>12.42567251460646</v>
+        <v>4.524026768922548</v>
       </c>
       <c r="K6" s="14" t="n"/>
       <c r="L6" s="14" t="n">
-        <v>13.13783480376886</v>
+        <v>2.801845126992966</v>
       </c>
       <c r="M6" s="14" t="n">
-        <v>12.38050782994369</v>
+        <v>4.501266270591698</v>
       </c>
       <c r="N6" s="13" t="n"/>
       <c r="O6" s="13" t="n"/>
@@ -2227,7 +2227,7 @@
         <v>2.844001213689403</v>
       </c>
       <c r="D7" s="14" t="n">
-        <v>9.703072181449262</v>
+        <v>5.328235491198823</v>
       </c>
       <c r="E7" s="14" t="n"/>
       <c r="F7" s="14" t="n">
@@ -2246,7 +2246,7 @@
         <v>2.296414533926163</v>
       </c>
       <c r="K7" s="14" t="n">
-        <v>13.13783480376886</v>
+        <v>2.801845126992966</v>
       </c>
       <c r="L7" s="14" t="n"/>
       <c r="M7" s="14" t="n">
@@ -2277,7 +2277,7 @@
         <v>0.1309988390392303</v>
       </c>
       <c r="D8" s="14" t="n">
-        <v>8.960981046584797</v>
+        <v>5.458721538855309</v>
       </c>
       <c r="E8" s="14" t="n">
         <v>2.72522560671845</v>
@@ -2295,7 +2295,7 @@
         <v>0.1053254352962912</v>
       </c>
       <c r="K8" s="14" t="n">
-        <v>12.38050782994369</v>
+        <v>4.501266270591698</v>
       </c>
       <c r="L8" s="14" t="n">
         <v>2.2572203961285</v>
@@ -2411,7 +2411,7 @@
         <v>0.2262904584572695</v>
       </c>
       <c r="D14" s="14" t="n">
-        <v>12.08381760429481</v>
+        <v>5.469262880668691</v>
       </c>
       <c r="E14" s="14" t="n">
         <v>2.701114701647342</v>
@@ -2429,7 +2429,7 @@
         <v>0.009103929232176572</v>
       </c>
       <c r="K14" s="14" t="n">
-        <v>0.474316134857282</v>
+        <v>0.3261869951982354</v>
       </c>
       <c r="L14" s="14" t="n">
         <v>0.005820922794185767</v>
@@ -2449,7 +2449,7 @@
       </c>
       <c r="C15" s="14" t="n"/>
       <c r="D15" s="14" t="n">
-        <v>12.04577796566226</v>
+        <v>5.497487840900265</v>
       </c>
       <c r="E15" s="14" t="n">
         <v>2.844001213689614</v>
@@ -2467,7 +2467,7 @@
       </c>
       <c r="J15" s="14" t="n"/>
       <c r="K15" s="14" t="n">
-        <v>0.465363295794745</v>
+        <v>0.3216644176543825</v>
       </c>
       <c r="L15" s="14" t="n">
         <v>0.003367651523479847</v>
@@ -2483,17 +2483,17 @@
         </is>
       </c>
       <c r="B16" s="14" t="n">
-        <v>12.08381760429481</v>
+        <v>5.469262880668691</v>
       </c>
       <c r="C16" s="14" t="n">
-        <v>12.04577796566226</v>
+        <v>5.497487840900265</v>
       </c>
       <c r="D16" s="14" t="n"/>
       <c r="E16" s="14" t="n">
-        <v>12.796691355624</v>
+        <v>5.328235491217509</v>
       </c>
       <c r="F16" s="14" t="n">
-        <v>12.09867764770548</v>
+        <v>5.458721538891282</v>
       </c>
       <c r="H16" s="12" t="inlineStr">
         <is>
@@ -2501,17 +2501,17 @@
         </is>
       </c>
       <c r="I16" s="14" t="n">
-        <v>0.474316134857282</v>
+        <v>0.3261869951982354</v>
       </c>
       <c r="J16" s="14" t="n">
-        <v>0.465363295794745</v>
+        <v>0.3216644176543825</v>
       </c>
       <c r="K16" s="14" t="n"/>
       <c r="L16" s="14" t="n">
-        <v>0.4687308738595936</v>
+        <v>0.3250320339686323</v>
       </c>
       <c r="M16" s="14" t="n">
-        <v>0.4701064277266727</v>
+        <v>0.3264076035532166</v>
       </c>
     </row>
     <row r="17" ht="15.85" customHeight="1" s="10">
@@ -2527,7 +2527,7 @@
         <v>2.844001213689614</v>
       </c>
       <c r="D17" s="14" t="n">
-        <v>12.796691355624</v>
+        <v>5.328235491217509</v>
       </c>
       <c r="E17" s="14" t="n"/>
       <c r="F17" s="14" t="n">
@@ -2545,7 +2545,7 @@
         <v>0.003367651523479847</v>
       </c>
       <c r="K17" s="14" t="n">
-        <v>0.4687308738595936</v>
+        <v>0.3250320339686323</v>
       </c>
       <c r="L17" s="14" t="n"/>
       <c r="M17" s="14" t="n">
@@ -2565,7 +2565,7 @@
         <v>0.1309988390130185</v>
       </c>
       <c r="D18" s="14" t="n">
-        <v>12.09867764770548</v>
+        <v>5.458721538891282</v>
       </c>
       <c r="E18" s="14" t="n">
         <v>2.725225606724025</v>
@@ -2583,7 +2583,7 @@
         <v>0.004743235699826326</v>
       </c>
       <c r="K18" s="14" t="n">
-        <v>0.4701064277266727</v>
+        <v>0.3264076035532166</v>
       </c>
       <c r="L18" s="14" t="n">
         <v>0.002265140801919659</v>

</xml_diff>

<commit_message>
updated specpess MP results with updated table
</commit_message>
<xml_diff>
--- a/results/comparison_table/Fishers_comparison.xlsx
+++ b/results/comparison_table/Fishers_comparison.xlsx
@@ -656,16 +656,16 @@
       </c>
       <c r="B4" s="14" t="n"/>
       <c r="C4" s="14" t="n">
-        <v>0.3773962335319018</v>
+        <v>0.37983151527761</v>
       </c>
       <c r="D4" s="14" t="n">
-        <v>9.919356917703732</v>
+        <v>7.44685327999801</v>
       </c>
       <c r="E4" s="14" t="n">
-        <v>4.689288745604718</v>
+        <v>4.689398169279855</v>
       </c>
       <c r="F4" s="14" t="n">
-        <v>0.5485364935722695</v>
+        <v>0.5534282731518388</v>
       </c>
       <c r="G4" s="13" t="n"/>
       <c r="H4" s="12" t="inlineStr">
@@ -675,16 +675,16 @@
       </c>
       <c r="I4" s="14" t="n"/>
       <c r="J4" s="14" t="n">
-        <v>0.35284833961881</v>
+        <v>0.3555149511842085</v>
       </c>
       <c r="K4" s="14" t="n">
-        <v>4.304025912258477</v>
+        <v>1.638660234711782</v>
       </c>
       <c r="L4" s="14" t="n">
-        <v>4.689288745605105</v>
+        <v>4.689398169292883</v>
       </c>
       <c r="M4" s="14" t="n">
-        <v>0.5518494451161595</v>
+        <v>0.555880910320297</v>
       </c>
       <c r="N4" s="13" t="n"/>
       <c r="O4" s="13" t="n"/>
@@ -705,17 +705,17 @@
         </is>
       </c>
       <c r="B5" s="14" t="n">
-        <v>0.3773962335319018</v>
+        <v>0.37983151527761</v>
       </c>
       <c r="C5" s="14" t="n"/>
       <c r="D5" s="14" t="n">
-        <v>9.886936539789014</v>
+        <v>7.402409024285747</v>
       </c>
       <c r="E5" s="14" t="n">
-        <v>4.719477185936323</v>
+        <v>4.719566996004048</v>
       </c>
       <c r="F5" s="14" t="n">
-        <v>0.1761392290294239</v>
+        <v>0.1772747619170639</v>
       </c>
       <c r="G5" s="13" t="n"/>
       <c r="H5" s="12" t="inlineStr">
@@ -724,17 +724,17 @@
         </is>
       </c>
       <c r="I5" s="14" t="n">
-        <v>0.35284833961881</v>
+        <v>0.3555149511842085</v>
       </c>
       <c r="J5" s="14" t="n"/>
       <c r="K5" s="14" t="n">
-        <v>3.981254205101203</v>
+        <v>1.630821204415821</v>
       </c>
       <c r="L5" s="14" t="n">
-        <v>4.719477185933972</v>
+        <v>4.719566996011725</v>
       </c>
       <c r="M5" s="14" t="n">
-        <v>0.2314736072303805</v>
+        <v>0.2329935306658965</v>
       </c>
       <c r="N5" s="13" t="n"/>
       <c r="O5" s="13" t="n"/>
@@ -755,17 +755,17 @@
         </is>
       </c>
       <c r="B6" s="14" t="n">
-        <v>9.919356917703732</v>
+        <v>7.44685327999801</v>
       </c>
       <c r="C6" s="14" t="n">
-        <v>9.886936539789014</v>
+        <v>7.402409024285747</v>
       </c>
       <c r="D6" s="14" t="n"/>
       <c r="E6" s="14" t="n">
-        <v>7.117976427563766</v>
+        <v>7.508599766439922</v>
       </c>
       <c r="F6" s="14" t="n">
-        <v>9.99217094197501</v>
+        <v>7.43725906158682</v>
       </c>
       <c r="G6" s="13" t="n"/>
       <c r="H6" s="12" t="inlineStr">
@@ -774,17 +774,17 @@
         </is>
       </c>
       <c r="I6" s="14" t="n">
-        <v>4.304025912258477</v>
+        <v>1.638660234711782</v>
       </c>
       <c r="J6" s="14" t="n">
-        <v>3.981254205101203</v>
+        <v>1.630821204415821</v>
       </c>
       <c r="K6" s="14" t="n"/>
       <c r="L6" s="14" t="n">
-        <v>5.106398705457906</v>
+        <v>5.150636344937815</v>
       </c>
       <c r="M6" s="14" t="n">
-        <v>3.930611463694983</v>
+        <v>1.657017485361074</v>
       </c>
       <c r="N6" s="13" t="n"/>
       <c r="O6" s="13" t="n"/>
@@ -805,17 +805,17 @@
         </is>
       </c>
       <c r="B7" s="14" t="n">
-        <v>4.689288745604718</v>
+        <v>4.689398169279855</v>
       </c>
       <c r="C7" s="14" t="n">
-        <v>4.719477185936323</v>
+        <v>4.719566996004048</v>
       </c>
       <c r="D7" s="14" t="n">
-        <v>7.117976427563766</v>
+        <v>7.508599766439922</v>
       </c>
       <c r="E7" s="14" t="n"/>
       <c r="F7" s="14" t="n">
-        <v>4.708879397782754</v>
+        <v>4.709004239008951</v>
       </c>
       <c r="G7" s="13" t="n"/>
       <c r="H7" s="12" t="inlineStr">
@@ -824,17 +824,17 @@
         </is>
       </c>
       <c r="I7" s="14" t="n">
-        <v>4.689288745605105</v>
+        <v>4.689398169292883</v>
       </c>
       <c r="J7" s="14" t="n">
-        <v>4.719477185933972</v>
+        <v>4.719566996011725</v>
       </c>
       <c r="K7" s="14" t="n">
-        <v>5.106398705457906</v>
+        <v>5.150636344937815</v>
       </c>
       <c r="L7" s="14" t="n"/>
       <c r="M7" s="14" t="n">
-        <v>4.7088793977721</v>
+        <v>4.70900423902857</v>
       </c>
       <c r="N7" s="13" t="n"/>
       <c r="O7" s="13" t="n"/>
@@ -855,16 +855,16 @@
         </is>
       </c>
       <c r="B8" s="14" t="n">
-        <v>0.5485364935722695</v>
+        <v>0.5534282731518388</v>
       </c>
       <c r="C8" s="14" t="n">
-        <v>0.1761392290294239</v>
+        <v>0.1772747619170639</v>
       </c>
       <c r="D8" s="14" t="n">
-        <v>9.99217094197501</v>
+        <v>7.43725906158682</v>
       </c>
       <c r="E8" s="14" t="n">
-        <v>4.708879397782754</v>
+        <v>4.709004239008951</v>
       </c>
       <c r="F8" s="14" t="n"/>
       <c r="H8" s="12" t="inlineStr">
@@ -873,16 +873,16 @@
         </is>
       </c>
       <c r="I8" s="14" t="n">
-        <v>0.5518494451161595</v>
+        <v>0.555880910320297</v>
       </c>
       <c r="J8" s="14" t="n">
-        <v>0.2314736072303805</v>
+        <v>0.2329935306658965</v>
       </c>
       <c r="K8" s="14" t="n">
-        <v>3.930611463694983</v>
+        <v>1.657017485361074</v>
       </c>
       <c r="L8" s="14" t="n">
-        <v>4.7088793977721</v>
+        <v>4.70900423902857</v>
       </c>
       <c r="M8" s="14" t="n"/>
     </row>
@@ -992,16 +992,16 @@
       </c>
       <c r="B14" s="14" t="n"/>
       <c r="C14" s="14" t="n">
-        <v>0.377396233533012</v>
+        <v>0.3798315152772271</v>
       </c>
       <c r="D14" s="14" t="n">
-        <v>9.919356917702338</v>
+        <v>7.446853279991807</v>
       </c>
       <c r="E14" s="14" t="n">
-        <v>3.186027703199337</v>
+        <v>3.186980209979991</v>
       </c>
       <c r="F14" s="14" t="n">
-        <v>0.5485364935734055</v>
+        <v>0.5534282731530721</v>
       </c>
       <c r="H14" s="12" t="inlineStr">
         <is>
@@ -1010,16 +1010,16 @@
       </c>
       <c r="I14" s="14" t="n"/>
       <c r="J14" s="14" t="n">
-        <v>0.002445764974182504</v>
+        <v>0.002427553292346711</v>
       </c>
       <c r="K14" s="14" t="n">
-        <v>4.264097540967208</v>
+        <v>1.251583407461038</v>
       </c>
       <c r="L14" s="14" t="n">
-        <v>0.005067295447965768</v>
+        <v>0.005034867410147947</v>
       </c>
       <c r="M14" s="14" t="n">
-        <v>0.004494523199528501</v>
+        <v>0.004466433469043626</v>
       </c>
     </row>
     <row r="15" ht="15.85" customHeight="1" s="10">
@@ -1029,17 +1029,17 @@
         </is>
       </c>
       <c r="B15" s="14" t="n">
-        <v>0.377396233533012</v>
+        <v>0.3798315152772271</v>
       </c>
       <c r="C15" s="14" t="n"/>
       <c r="D15" s="14" t="n">
-        <v>9.886936539793002</v>
+        <v>7.402409024286854</v>
       </c>
       <c r="E15" s="14" t="n">
-        <v>3.15331911680175</v>
+        <v>3.155452042715881</v>
       </c>
       <c r="F15" s="14" t="n">
-        <v>0.1761392290301824</v>
+        <v>0.1772747619180322</v>
       </c>
       <c r="H15" s="12" t="inlineStr">
         <is>
@@ -1047,17 +1047,17 @@
         </is>
       </c>
       <c r="I15" s="14" t="n">
-        <v>0.002445764974182504</v>
+        <v>0.002427553292346711</v>
       </c>
       <c r="J15" s="14" t="n"/>
       <c r="K15" s="14" t="n">
-        <v>4.265870609220072</v>
+        <v>1.251648196521558</v>
       </c>
       <c r="L15" s="14" t="n">
-        <v>0.003617750813900871</v>
+        <v>0.003553046648408649</v>
       </c>
       <c r="M15" s="14" t="n">
-        <v>0.002821980829311123</v>
+        <v>0.0027651938610264</v>
       </c>
     </row>
     <row r="16" ht="15.85" customHeight="1" s="10">
@@ -1067,17 +1067,17 @@
         </is>
       </c>
       <c r="B16" s="14" t="n">
-        <v>9.919356917702338</v>
+        <v>7.446853279991807</v>
       </c>
       <c r="C16" s="14" t="n">
-        <v>9.886936539793002</v>
+        <v>7.402409024286854</v>
       </c>
       <c r="D16" s="14" t="n"/>
       <c r="E16" s="14" t="n">
-        <v>7.117976427563251</v>
+        <v>7.508599766440905</v>
       </c>
       <c r="F16" s="14" t="n">
-        <v>9.992170941966545</v>
+        <v>7.43725906158266</v>
       </c>
       <c r="H16" s="12" t="inlineStr">
         <is>
@@ -1085,17 +1085,17 @@
         </is>
       </c>
       <c r="I16" s="14" t="n">
-        <v>4.264097540967208</v>
+        <v>1.251583407461038</v>
       </c>
       <c r="J16" s="14" t="n">
-        <v>4.265870609220072</v>
+        <v>1.251648196521558</v>
       </c>
       <c r="K16" s="14" t="n"/>
       <c r="L16" s="14" t="n">
-        <v>4.269155611861901</v>
+        <v>1.249225073247839</v>
       </c>
       <c r="M16" s="14" t="n">
-        <v>4.26838847448473</v>
+        <v>1.250475563523088</v>
       </c>
     </row>
     <row r="17" ht="15.85" customHeight="1" s="10">
@@ -1105,17 +1105,17 @@
         </is>
       </c>
       <c r="B17" s="14" t="n">
-        <v>3.186027703199337</v>
+        <v>3.186980209979991</v>
       </c>
       <c r="C17" s="14" t="n">
-        <v>3.15331911680175</v>
+        <v>3.155452042715881</v>
       </c>
       <c r="D17" s="14" t="n">
-        <v>7.117976427563251</v>
+        <v>7.508599766440905</v>
       </c>
       <c r="E17" s="14" t="n"/>
       <c r="F17" s="14" t="n">
-        <v>3.259494281966406</v>
+        <v>3.262576215529002</v>
       </c>
       <c r="H17" s="12" t="inlineStr">
         <is>
@@ -1123,17 +1123,17 @@
         </is>
       </c>
       <c r="I17" s="14" t="n">
-        <v>0.005067295447965768</v>
+        <v>0.005034867410147947</v>
       </c>
       <c r="J17" s="14" t="n">
-        <v>0.003617750813900871</v>
+        <v>0.003553046648408649</v>
       </c>
       <c r="K17" s="14" t="n">
-        <v>4.269155611861901</v>
+        <v>1.249225073247839</v>
       </c>
       <c r="L17" s="14" t="n"/>
       <c r="M17" s="14" t="n">
-        <v>0.001250791272115822</v>
+        <v>0.001250685647740378</v>
       </c>
     </row>
     <row r="18" ht="15.85" customHeight="1" s="10">
@@ -1143,16 +1143,16 @@
         </is>
       </c>
       <c r="B18" s="14" t="n">
-        <v>0.5485364935734055</v>
+        <v>0.5534282731530721</v>
       </c>
       <c r="C18" s="14" t="n">
-        <v>0.1761392290301824</v>
+        <v>0.1772747619180322</v>
       </c>
       <c r="D18" s="14" t="n">
-        <v>9.992170941966545</v>
+        <v>7.43725906158266</v>
       </c>
       <c r="E18" s="14" t="n">
-        <v>3.259494281966406</v>
+        <v>3.262576215529002</v>
       </c>
       <c r="F18" s="14" t="n"/>
       <c r="H18" s="12" t="inlineStr">
@@ -1161,16 +1161,16 @@
         </is>
       </c>
       <c r="I18" s="14" t="n">
-        <v>0.004494523199528501</v>
+        <v>0.004466433469043626</v>
       </c>
       <c r="J18" s="14" t="n">
-        <v>0.002821980829311123</v>
+        <v>0.0027651938610264</v>
       </c>
       <c r="K18" s="14" t="n">
-        <v>4.26838847448473</v>
+        <v>1.250475563523088</v>
       </c>
       <c r="L18" s="14" t="n">
-        <v>0.001250791272115822</v>
+        <v>0.001250685647740378</v>
       </c>
       <c r="M18" s="14" t="n"/>
     </row>
@@ -1364,16 +1364,16 @@
       </c>
       <c r="B4" s="14" t="n"/>
       <c r="C4" s="14" t="n">
-        <v>0.3726463025137923</v>
+        <v>0.3737543076736359</v>
       </c>
       <c r="D4" s="14" t="n">
         <v>3.384266125046481</v>
       </c>
       <c r="E4" s="14" t="n">
-        <v>1.173174098906264</v>
+        <v>1.167671321938141</v>
       </c>
       <c r="F4" s="14" t="n">
-        <v>0.4808059913145969</v>
+        <v>0.481850568863881</v>
       </c>
       <c r="G4" s="13" t="n"/>
       <c r="H4" s="12" t="inlineStr">
@@ -1383,16 +1383,16 @@
       </c>
       <c r="I4" s="14" t="n"/>
       <c r="J4" s="14" t="n">
-        <v>0.4491435128481215</v>
+        <v>0.4492894982635293</v>
       </c>
       <c r="K4" s="14" t="n">
         <v>1.189449767637524</v>
       </c>
       <c r="L4" s="14" t="n">
-        <v>2.865230972178754</v>
+        <v>2.866247623522129</v>
       </c>
       <c r="M4" s="14" t="n">
-        <v>0.5774622991955048</v>
+        <v>0.5775403457419029</v>
       </c>
       <c r="N4" s="13" t="n"/>
       <c r="O4" s="13" t="n"/>
@@ -1413,17 +1413,17 @@
         </is>
       </c>
       <c r="B5" s="14" t="n">
-        <v>0.3726463025137923</v>
+        <v>0.3737543076736359</v>
       </c>
       <c r="C5" s="14" t="n"/>
       <c r="D5" s="14" t="n">
-        <v>3.918593313466014</v>
+        <v>3.388220223339327</v>
       </c>
       <c r="E5" s="14" t="n">
-        <v>1.314870456468473</v>
+        <v>1.323146899176907</v>
       </c>
       <c r="F5" s="14" t="n">
-        <v>0.1081616267389053</v>
+        <v>0.1080982079711638</v>
       </c>
       <c r="G5" s="13" t="n"/>
       <c r="H5" s="12" t="inlineStr">
@@ -1432,17 +1432,17 @@
         </is>
       </c>
       <c r="I5" s="14" t="n">
-        <v>0.4491435128481215</v>
+        <v>0.4492894982635293</v>
       </c>
       <c r="J5" s="14" t="n"/>
       <c r="K5" s="14" t="n">
-        <v>1.202402704743217</v>
+        <v>1.202574220265918</v>
       </c>
       <c r="L5" s="14" t="n">
-        <v>2.88437463456303</v>
+        <v>2.885390970875982</v>
       </c>
       <c r="M5" s="14" t="n">
-        <v>0.1392586598233071</v>
+        <v>0.1391524676045001</v>
       </c>
       <c r="N5" s="13" t="n"/>
       <c r="O5" s="13" t="n"/>
@@ -1466,14 +1466,14 @@
         <v>3.384266125046481</v>
       </c>
       <c r="C6" s="14" t="n">
-        <v>3.918593313466014</v>
+        <v>3.388220223339327</v>
       </c>
       <c r="D6" s="14" t="n"/>
       <c r="E6" s="14" t="n">
-        <v>4.242445508897008</v>
+        <v>3.697495070373798</v>
       </c>
       <c r="F6" s="14" t="n">
-        <v>10.84918233753177</v>
+        <v>3.402226655773111</v>
       </c>
       <c r="G6" s="13" t="n"/>
       <c r="H6" s="12" t="inlineStr">
@@ -1485,14 +1485,14 @@
         <v>1.189449767637524</v>
       </c>
       <c r="J6" s="14" t="n">
-        <v>1.202402704743217</v>
+        <v>1.202574220265918</v>
       </c>
       <c r="K6" s="14" t="n"/>
       <c r="L6" s="14" t="n">
-        <v>1.636833993271819</v>
+        <v>1.70824020268777</v>
       </c>
       <c r="M6" s="14" t="n">
-        <v>2.617148387586216</v>
+        <v>1.269127300816686</v>
       </c>
       <c r="N6" s="13" t="n"/>
       <c r="O6" s="13" t="n"/>
@@ -1513,17 +1513,17 @@
         </is>
       </c>
       <c r="B7" s="14" t="n">
-        <v>1.173174098906264</v>
+        <v>1.167671321938141</v>
       </c>
       <c r="C7" s="14" t="n">
-        <v>1.314870456468473</v>
+        <v>1.323146899176907</v>
       </c>
       <c r="D7" s="14" t="n">
-        <v>4.242445508897008</v>
+        <v>3.697495070373798</v>
       </c>
       <c r="E7" s="14" t="n"/>
       <c r="F7" s="14" t="n">
-        <v>1.260488548518442</v>
+        <v>1.26839289298561</v>
       </c>
       <c r="G7" s="13" t="n"/>
       <c r="H7" s="12" t="inlineStr">
@@ -1532,17 +1532,17 @@
         </is>
       </c>
       <c r="I7" s="14" t="n">
-        <v>2.865230972178754</v>
+        <v>2.866247623522129</v>
       </c>
       <c r="J7" s="14" t="n">
-        <v>2.88437463456303</v>
+        <v>2.885390970875982</v>
       </c>
       <c r="K7" s="14" t="n">
-        <v>1.636833993271819</v>
+        <v>1.70824020268777</v>
       </c>
       <c r="L7" s="14" t="n"/>
       <c r="M7" s="14" t="n">
-        <v>2.97560847582311</v>
+        <v>2.976722157797494</v>
       </c>
       <c r="N7" s="13" t="n"/>
       <c r="O7" s="13" t="n"/>
@@ -1563,16 +1563,16 @@
         </is>
       </c>
       <c r="B8" s="14" t="n">
-        <v>0.4808059913145969</v>
+        <v>0.481850568863881</v>
       </c>
       <c r="C8" s="14" t="n">
-        <v>0.1081616267389053</v>
+        <v>0.1080982079711638</v>
       </c>
       <c r="D8" s="14" t="n">
-        <v>10.84918233753177</v>
+        <v>3.402226655773111</v>
       </c>
       <c r="E8" s="14" t="n">
-        <v>1.260488548518442</v>
+        <v>1.26839289298561</v>
       </c>
       <c r="F8" s="14" t="n"/>
       <c r="H8" s="12" t="inlineStr">
@@ -1581,16 +1581,16 @@
         </is>
       </c>
       <c r="I8" s="14" t="n">
-        <v>0.5774622991955048</v>
+        <v>0.5775403457419029</v>
       </c>
       <c r="J8" s="14" t="n">
-        <v>0.1392586598233071</v>
+        <v>0.1391524676045001</v>
       </c>
       <c r="K8" s="14" t="n">
-        <v>2.617148387586216</v>
+        <v>1.269127300816686</v>
       </c>
       <c r="L8" s="14" t="n">
-        <v>2.97560847582311</v>
+        <v>2.976722157797494</v>
       </c>
       <c r="M8" s="14" t="n"/>
     </row>
@@ -1700,16 +1700,16 @@
       </c>
       <c r="B14" s="14" t="n"/>
       <c r="C14" s="14" t="n">
-        <v>0.3726463025141316</v>
+        <v>0.3737543076731272</v>
       </c>
       <c r="D14" s="14" t="n">
         <v>3.38426612505494</v>
       </c>
       <c r="E14" s="14" t="n">
-        <v>2.081437496736004</v>
+        <v>2.075664157119447</v>
       </c>
       <c r="F14" s="14" t="n">
-        <v>0.4808059913156109</v>
+        <v>0.4818505688625467</v>
       </c>
       <c r="H14" s="12" t="inlineStr">
         <is>
@@ -1718,16 +1718,16 @@
       </c>
       <c r="I14" s="14" t="n"/>
       <c r="J14" s="14" t="n">
-        <v>0.004883347111689611</v>
+        <v>0.004882949690554564</v>
       </c>
       <c r="K14" s="14" t="n">
-        <v>1.592455224818253</v>
+        <v>1.592455224819079</v>
       </c>
       <c r="L14" s="14" t="n">
-        <v>0.005149342423874624</v>
+        <v>0.005148485663070614</v>
       </c>
       <c r="M14" s="14" t="n">
-        <v>0.006224795222596624</v>
+        <v>0.006224243235476163</v>
       </c>
     </row>
     <row r="15" ht="15.85" customHeight="1" s="10">
@@ -1737,17 +1737,17 @@
         </is>
       </c>
       <c r="B15" s="14" t="n">
-        <v>0.3726463025141316</v>
+        <v>0.3737543076731272</v>
       </c>
       <c r="C15" s="14" t="n"/>
       <c r="D15" s="14" t="n">
-        <v>3.62054734826109</v>
+        <v>3.388220223344394</v>
       </c>
       <c r="E15" s="14" t="n">
-        <v>2.106366134259678</v>
+        <v>2.100661917745584</v>
       </c>
       <c r="F15" s="14" t="n">
-        <v>0.1081616267395801</v>
+        <v>0.1080982079703218</v>
       </c>
       <c r="H15" s="12" t="inlineStr">
         <is>
@@ -1755,17 +1755,17 @@
         </is>
       </c>
       <c r="I15" s="14" t="n">
-        <v>0.004883347111689611</v>
+        <v>0.004882949690554564</v>
       </c>
       <c r="J15" s="14" t="n"/>
       <c r="K15" s="14" t="n">
-        <v>4.097090025903984</v>
+        <v>1.596249215629797</v>
       </c>
       <c r="L15" s="14" t="n">
-        <v>0.001263305374658307</v>
+        <v>0.001233016899913078</v>
       </c>
       <c r="M15" s="14" t="n">
-        <v>0.001359305145372738</v>
+        <v>0.001359158153758729</v>
       </c>
     </row>
     <row r="16" ht="15.85" customHeight="1" s="10">
@@ -1778,14 +1778,14 @@
         <v>3.38426612505494</v>
       </c>
       <c r="C16" s="14" t="n">
-        <v>3.62054734826109</v>
+        <v>3.388220223344394</v>
       </c>
       <c r="D16" s="14" t="n"/>
       <c r="E16" s="14" t="n">
-        <v>4.242445508900473</v>
+        <v>3.697495070378792</v>
       </c>
       <c r="F16" s="14" t="n">
-        <v>10.84918233753237</v>
+        <v>3.402226655778946</v>
       </c>
       <c r="H16" s="12" t="inlineStr">
         <is>
@@ -1793,17 +1793,17 @@
         </is>
       </c>
       <c r="I16" s="14" t="n">
-        <v>1.592455224818253</v>
+        <v>1.592455224819079</v>
       </c>
       <c r="J16" s="14" t="n">
-        <v>4.097090025903984</v>
+        <v>1.596249215629797</v>
       </c>
       <c r="K16" s="14" t="n"/>
       <c r="L16" s="14" t="n">
-        <v>4.09713449033247</v>
+        <v>1.596431806717735</v>
       </c>
       <c r="M16" s="14" t="n">
-        <v>3.454313084573598</v>
+        <v>1.597460369086904</v>
       </c>
     </row>
     <row r="17" ht="15.85" customHeight="1" s="10">
@@ -1813,17 +1813,17 @@
         </is>
       </c>
       <c r="B17" s="14" t="n">
-        <v>2.081437496736004</v>
+        <v>2.075664157119447</v>
       </c>
       <c r="C17" s="14" t="n">
-        <v>2.106366134259678</v>
+        <v>2.100661917745584</v>
       </c>
       <c r="D17" s="14" t="n">
-        <v>4.242445508900473</v>
+        <v>3.697495070378792</v>
       </c>
       <c r="E17" s="14" t="n"/>
       <c r="F17" s="14" t="n">
-        <v>2.104415939014535</v>
+        <v>2.098683267589815</v>
       </c>
       <c r="H17" s="12" t="inlineStr">
         <is>
@@ -1831,17 +1831,17 @@
         </is>
       </c>
       <c r="I17" s="14" t="n">
-        <v>0.005149342423874624</v>
+        <v>0.005148485663070614</v>
       </c>
       <c r="J17" s="14" t="n">
-        <v>0.001263305374658307</v>
+        <v>0.001233016899913078</v>
       </c>
       <c r="K17" s="14" t="n">
-        <v>4.09713449033247</v>
+        <v>1.596431806717735</v>
       </c>
       <c r="L17" s="14" t="n"/>
       <c r="M17" s="14" t="n">
-        <v>0.001075452800861554</v>
+        <v>0.001075757575421001</v>
       </c>
     </row>
     <row r="18" ht="15.85" customHeight="1" s="10">
@@ -1851,16 +1851,16 @@
         </is>
       </c>
       <c r="B18" s="14" t="n">
-        <v>0.4808059913156109</v>
+        <v>0.4818505688625467</v>
       </c>
       <c r="C18" s="14" t="n">
-        <v>0.1081616267395801</v>
+        <v>0.1080982079703218</v>
       </c>
       <c r="D18" s="14" t="n">
-        <v>10.84918233753237</v>
+        <v>3.402226655778946</v>
       </c>
       <c r="E18" s="14" t="n">
-        <v>2.104415939014535</v>
+        <v>2.098683267589815</v>
       </c>
       <c r="F18" s="14" t="n"/>
       <c r="H18" s="12" t="inlineStr">
@@ -1869,16 +1869,16 @@
         </is>
       </c>
       <c r="I18" s="14" t="n">
-        <v>0.006224795222596624</v>
+        <v>0.006224243235476163</v>
       </c>
       <c r="J18" s="14" t="n">
-        <v>0.001359305145372738</v>
+        <v>0.001359158153758729</v>
       </c>
       <c r="K18" s="14" t="n">
-        <v>3.454313084573598</v>
+        <v>1.597460369086904</v>
       </c>
       <c r="L18" s="14" t="n">
-        <v>0.001075452800861554</v>
+        <v>0.001075757575421001</v>
       </c>
       <c r="M18" s="14" t="n"/>
     </row>
@@ -2072,16 +2072,16 @@
       </c>
       <c r="B4" s="14" t="n"/>
       <c r="C4" s="14" t="n">
-        <v>0.2262904584537549</v>
+        <v>0.4755238534890436</v>
       </c>
       <c r="D4" s="14" t="n">
         <v>5.469262880664999</v>
       </c>
       <c r="E4" s="14" t="n">
-        <v>2.701114701640339</v>
+        <v>2.557290407849714</v>
       </c>
       <c r="F4" s="14" t="n">
-        <v>0.1144526964760178</v>
+        <v>0.3445271606153611</v>
       </c>
       <c r="G4" s="13" t="n"/>
       <c r="H4" s="12" t="inlineStr">
@@ -2091,16 +2091,16 @@
       </c>
       <c r="I4" s="14" t="n"/>
       <c r="J4" s="14" t="n">
-        <v>0.09070967271611728</v>
+        <v>0.1767080622250866</v>
       </c>
       <c r="K4" s="14" t="n">
         <v>4.519503360644053</v>
       </c>
       <c r="L4" s="14" t="n">
-        <v>2.274282554125683</v>
+        <v>2.268560988172997</v>
       </c>
       <c r="M4" s="14" t="n">
-        <v>0.1960349207199441</v>
+        <v>0.2820329726057389</v>
       </c>
       <c r="N4" s="13" t="n"/>
       <c r="O4" s="13" t="n"/>
@@ -2121,7 +2121,7 @@
         </is>
       </c>
       <c r="B5" s="14" t="n">
-        <v>0.2262904584537549</v>
+        <v>0.4755238534890436</v>
       </c>
       <c r="C5" s="14" t="n"/>
       <c r="D5" s="14" t="n">
@@ -2140,7 +2140,7 @@
         </is>
       </c>
       <c r="I5" s="14" t="n">
-        <v>0.09070967271611728</v>
+        <v>0.1767080622250866</v>
       </c>
       <c r="J5" s="14" t="n"/>
       <c r="K5" s="14" t="n">
@@ -2221,7 +2221,7 @@
         </is>
       </c>
       <c r="B7" s="14" t="n">
-        <v>2.701114701640339</v>
+        <v>2.557290407849714</v>
       </c>
       <c r="C7" s="14" t="n">
         <v>2.844001213689403</v>
@@ -2240,7 +2240,7 @@
         </is>
       </c>
       <c r="I7" s="14" t="n">
-        <v>2.274282554125683</v>
+        <v>2.268560988172997</v>
       </c>
       <c r="J7" s="14" t="n">
         <v>2.296414533926163</v>
@@ -2271,7 +2271,7 @@
         </is>
       </c>
       <c r="B8" s="14" t="n">
-        <v>0.1144526964760178</v>
+        <v>0.3445271606153611</v>
       </c>
       <c r="C8" s="14" t="n">
         <v>0.1309988390392303</v>
@@ -2289,7 +2289,7 @@
         </is>
       </c>
       <c r="I8" s="14" t="n">
-        <v>0.1960349207199441</v>
+        <v>0.2820329726057389</v>
       </c>
       <c r="J8" s="14" t="n">
         <v>0.1053254352962912</v>
@@ -2408,16 +2408,16 @@
       </c>
       <c r="B14" s="14" t="n"/>
       <c r="C14" s="14" t="n">
-        <v>0.2262904584572695</v>
+        <v>0.4755238534801394</v>
       </c>
       <c r="D14" s="14" t="n">
         <v>5.469262880668691</v>
       </c>
       <c r="E14" s="14" t="n">
-        <v>2.701114701647342</v>
+        <v>2.557290407850316</v>
       </c>
       <c r="F14" s="14" t="n">
-        <v>0.1231076356932917</v>
+        <v>0.3445271606326816</v>
       </c>
       <c r="H14" s="12" t="inlineStr">
         <is>
@@ -2426,16 +2426,16 @@
       </c>
       <c r="I14" s="14" t="n"/>
       <c r="J14" s="14" t="n">
-        <v>0.009103929232176572</v>
+        <v>0.01209734535177153</v>
       </c>
       <c r="K14" s="14" t="n">
         <v>0.3261869951982354</v>
       </c>
       <c r="L14" s="14" t="n">
-        <v>0.005820922794185767</v>
+        <v>0.01005447058395561</v>
       </c>
       <c r="M14" s="14" t="n">
-        <v>0.005322797304849306</v>
+        <v>0.01188115524884015</v>
       </c>
     </row>
     <row r="15" ht="15.85" customHeight="1" s="10">
@@ -2445,7 +2445,7 @@
         </is>
       </c>
       <c r="B15" s="14" t="n">
-        <v>0.2262904584572695</v>
+        <v>0.4755238534801394</v>
       </c>
       <c r="C15" s="14" t="n"/>
       <c r="D15" s="14" t="n">
@@ -2463,11 +2463,11 @@
         </is>
       </c>
       <c r="I15" s="14" t="n">
-        <v>0.009103929232176572</v>
+        <v>0.01209734535177153</v>
       </c>
       <c r="J15" s="14" t="n"/>
       <c r="K15" s="14" t="n">
-        <v>0.3216644176543825</v>
+        <v>0.3216644176543667</v>
       </c>
       <c r="L15" s="14" t="n">
         <v>0.003367651523479847</v>
@@ -2504,11 +2504,11 @@
         <v>0.3261869951982354</v>
       </c>
       <c r="J16" s="14" t="n">
-        <v>0.3216644176543825</v>
+        <v>0.3216644176543667</v>
       </c>
       <c r="K16" s="14" t="n"/>
       <c r="L16" s="14" t="n">
-        <v>0.3250320339686323</v>
+        <v>0.3250320339686322</v>
       </c>
       <c r="M16" s="14" t="n">
         <v>0.3264076035532166</v>
@@ -2521,7 +2521,7 @@
         </is>
       </c>
       <c r="B17" s="14" t="n">
-        <v>2.701114701647342</v>
+        <v>2.557290407850316</v>
       </c>
       <c r="C17" s="14" t="n">
         <v>2.844001213689614</v>
@@ -2539,13 +2539,13 @@
         </is>
       </c>
       <c r="I17" s="14" t="n">
-        <v>0.005820922794185767</v>
+        <v>0.01005447058395561</v>
       </c>
       <c r="J17" s="14" t="n">
         <v>0.003367651523479847</v>
       </c>
       <c r="K17" s="14" t="n">
-        <v>0.3250320339686323</v>
+        <v>0.3250320339686322</v>
       </c>
       <c r="L17" s="14" t="n"/>
       <c r="M17" s="14" t="n">
@@ -2559,7 +2559,7 @@
         </is>
       </c>
       <c r="B18" s="14" t="n">
-        <v>0.1231076356932917</v>
+        <v>0.3445271606326816</v>
       </c>
       <c r="C18" s="14" t="n">
         <v>0.1309988390130185</v>
@@ -2577,7 +2577,7 @@
         </is>
       </c>
       <c r="I18" s="14" t="n">
-        <v>0.005322797304849306</v>
+        <v>0.01188115524884015</v>
       </c>
       <c r="J18" s="14" t="n">
         <v>0.004743235699826326</v>
@@ -2783,7 +2783,7 @@
         <v>0.06211140463036885</v>
       </c>
       <c r="D4" s="14" t="n">
-        <v>8.062588612130609</v>
+        <v>4.825168498861247</v>
       </c>
       <c r="E4" s="14" t="n">
         <v>2.874882720546051</v>
@@ -2802,7 +2802,7 @@
         <v>0.1030983777729827</v>
       </c>
       <c r="K4" s="14" t="n">
-        <v>10.48676195248214</v>
+        <v>4.3222372578501</v>
       </c>
       <c r="L4" s="14" t="n">
         <v>2.908151926234752</v>
@@ -2833,7 +2833,7 @@
       </c>
       <c r="C5" s="14" t="n"/>
       <c r="D5" s="14" t="n">
-        <v>8.006569333036184</v>
+        <v>4.850030810431934</v>
       </c>
       <c r="E5" s="14" t="n">
         <v>2.935483613418856</v>
@@ -2852,7 +2852,7 @@
       </c>
       <c r="J5" s="14" t="n"/>
       <c r="K5" s="14" t="n">
-        <v>10.47856220274357</v>
+        <v>4.418911732640574</v>
       </c>
       <c r="L5" s="14" t="n">
         <v>3.001984560012908</v>
@@ -2879,17 +2879,17 @@
         </is>
       </c>
       <c r="B6" s="14" t="n">
-        <v>8.062588612130609</v>
+        <v>4.825168498861247</v>
       </c>
       <c r="C6" s="14" t="n">
-        <v>8.006569333036184</v>
+        <v>4.850030810431934</v>
       </c>
       <c r="D6" s="14" t="n"/>
       <c r="E6" s="14" t="n">
-        <v>8.856491601352039</v>
+        <v>4.574473111199865</v>
       </c>
       <c r="F6" s="14" t="n">
-        <v>7.859104476890197</v>
+        <v>4.830005025486532</v>
       </c>
       <c r="G6" s="13" t="n"/>
       <c r="H6" s="12" t="inlineStr">
@@ -2898,17 +2898,17 @@
         </is>
       </c>
       <c r="I6" s="14" t="n">
-        <v>10.48676195248214</v>
+        <v>4.3222372578501</v>
       </c>
       <c r="J6" s="14" t="n">
-        <v>10.47856220274357</v>
+        <v>4.418911732640574</v>
       </c>
       <c r="K6" s="14" t="n"/>
       <c r="L6" s="14" t="n">
-        <v>11.20511984687745</v>
+        <v>3.061000783310165</v>
       </c>
       <c r="M6" s="14" t="n">
-        <v>10.43795098231388</v>
+        <v>4.385584440343489</v>
       </c>
       <c r="N6" s="13" t="n"/>
       <c r="O6" s="13" t="n"/>
@@ -2935,7 +2935,7 @@
         <v>2.935483613418856</v>
       </c>
       <c r="D7" s="14" t="n">
-        <v>8.856491601352039</v>
+        <v>4.574473111199865</v>
       </c>
       <c r="E7" s="14" t="n"/>
       <c r="F7" s="14" t="n">
@@ -2954,7 +2954,7 @@
         <v>3.001984560012908</v>
       </c>
       <c r="K7" s="14" t="n">
-        <v>11.20511984687745</v>
+        <v>3.061000783310165</v>
       </c>
       <c r="L7" s="14" t="n"/>
       <c r="M7" s="14" t="n">
@@ -2985,7 +2985,7 @@
         <v>0.2263305621388694</v>
       </c>
       <c r="D8" s="14" t="n">
-        <v>7.859104476890197</v>
+        <v>4.830005025486532</v>
       </c>
       <c r="E8" s="14" t="n">
         <v>2.749203952310937</v>
@@ -3003,7 +3003,7 @@
         <v>0.0838425850827151</v>
       </c>
       <c r="K8" s="14" t="n">
-        <v>10.43795098231388</v>
+        <v>4.385584440343489</v>
       </c>
       <c r="L8" s="14" t="n">
         <v>2.957255371749487</v>
@@ -3119,7 +3119,7 @@
         <v>0.07873614082986091</v>
       </c>
       <c r="D14" s="14" t="n">
-        <v>11.69423127716002</v>
+        <v>4.825168498847844</v>
       </c>
       <c r="E14" s="14" t="n">
         <v>2.874882720540283</v>
@@ -3137,10 +3137,10 @@
         <v>0.009000578402860821</v>
       </c>
       <c r="K14" s="14" t="n">
-        <v>0.3068155992074563</v>
+        <v>0.2387058801276417</v>
       </c>
       <c r="L14" s="14" t="n">
-        <v>0.00584734573916154</v>
+        <v>0.005847345739131406</v>
       </c>
       <c r="M14" s="14" t="n">
         <v>0.00668911770624058</v>
@@ -3157,7 +3157,7 @@
       </c>
       <c r="C15" s="14" t="n"/>
       <c r="D15" s="14" t="n">
-        <v>11.6573241284687</v>
+        <v>4.850030810465669</v>
       </c>
       <c r="E15" s="14" t="n">
         <v>2.935483613414252</v>
@@ -3175,10 +3175,10 @@
       </c>
       <c r="J15" s="14" t="n"/>
       <c r="K15" s="14" t="n">
-        <v>0.2983315187058641</v>
+        <v>0.2302217685931421</v>
       </c>
       <c r="L15" s="14" t="n">
-        <v>0.003200027864232041</v>
+        <v>0.003200027864261418</v>
       </c>
       <c r="M15" s="14" t="n">
         <v>0.00418353106395057</v>
@@ -3191,17 +3191,17 @@
         </is>
       </c>
       <c r="B16" s="14" t="n">
-        <v>11.69423127716002</v>
+        <v>4.825168498847844</v>
       </c>
       <c r="C16" s="14" t="n">
-        <v>11.6573241284687</v>
+        <v>4.850030810465669</v>
       </c>
       <c r="D16" s="14" t="n"/>
       <c r="E16" s="14" t="n">
-        <v>12.47793868942139</v>
+        <v>4.574473111197271</v>
       </c>
       <c r="F16" s="14" t="n">
-        <v>11.72636687679834</v>
+        <v>4.830005025475884</v>
       </c>
       <c r="H16" s="12" t="inlineStr">
         <is>
@@ -3209,17 +3209,17 @@
         </is>
       </c>
       <c r="I16" s="14" t="n">
-        <v>0.3068155992074563</v>
+        <v>0.2387058801276417</v>
       </c>
       <c r="J16" s="14" t="n">
-        <v>0.2983315187058641</v>
+        <v>0.2302217685931421</v>
       </c>
       <c r="K16" s="14" t="n"/>
       <c r="L16" s="14" t="n">
-        <v>0.3011553713424278</v>
+        <v>0.2330456314498744</v>
       </c>
       <c r="M16" s="14" t="n">
-        <v>0.3025150120135459</v>
+        <v>0.2344052770805847</v>
       </c>
     </row>
     <row r="17" ht="15.85" customHeight="1" s="10">
@@ -3235,7 +3235,7 @@
         <v>2.935483613414252</v>
       </c>
       <c r="D17" s="14" t="n">
-        <v>12.47793868942139</v>
+        <v>4.574473111197271</v>
       </c>
       <c r="E17" s="14" t="n"/>
       <c r="F17" s="14" t="n">
@@ -3247,17 +3247,17 @@
         </is>
       </c>
       <c r="I17" s="14" t="n">
-        <v>0.00584734573916154</v>
+        <v>0.005847345739131406</v>
       </c>
       <c r="J17" s="14" t="n">
-        <v>0.003200027864232041</v>
+        <v>0.003200027864261418</v>
       </c>
       <c r="K17" s="14" t="n">
-        <v>0.3011553713424278</v>
+        <v>0.2330456314498744</v>
       </c>
       <c r="L17" s="14" t="n"/>
       <c r="M17" s="14" t="n">
-        <v>0.001997812498847041</v>
+        <v>0.001997812498867454</v>
       </c>
     </row>
     <row r="18" ht="15.85" customHeight="1" s="10">
@@ -3273,7 +3273,7 @@
         <v>0.2263305621488368</v>
       </c>
       <c r="D18" s="14" t="n">
-        <v>11.72636687679834</v>
+        <v>4.830005025475884</v>
       </c>
       <c r="E18" s="14" t="n">
         <v>2.749203952297027</v>
@@ -3291,10 +3291,10 @@
         <v>0.00418353106395057</v>
       </c>
       <c r="K18" s="14" t="n">
-        <v>0.3025150120135459</v>
+        <v>0.2344052770805847</v>
       </c>
       <c r="L18" s="14" t="n">
-        <v>0.001997812498847041</v>
+        <v>0.001997812498867454</v>
       </c>
       <c r="M18" s="14" t="n"/>
     </row>

</xml_diff>